<commit_message>
Mise à jour de la documentation du projet
</commit_message>
<xml_diff>
--- a/ClasseurAnalyseSiteWeb-Rossello-Rodrigue-Lebagousse.xlsx
+++ b/ClasseurAnalyseSiteWeb-Rossello-Rodrigue-Lebagousse.xlsx
@@ -9,20 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="EXIGENCES" sheetId="1" r:id="rId1"/>
     <sheet name="PARTICIPANTS" sheetId="2" r:id="rId2"/>
     <sheet name="Estimation" sheetId="3" r:id="rId3"/>
-    <sheet name="MATRICE DE TRACABILITE" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>EXIGENCES</t>
   </si>
@@ -69,24 +68,6 @@
     <t>APPROBATEUR</t>
   </si>
   <si>
-    <t>TESTS / EXIGENCES</t>
-  </si>
-  <si>
-    <t>EXIGENCE N°</t>
-  </si>
-  <si>
-    <t>TEST N°</t>
-  </si>
-  <si>
-    <t>STATUS</t>
-  </si>
-  <si>
-    <t>RESULTAT (OK/KO)</t>
-  </si>
-  <si>
-    <t>BUG ID</t>
-  </si>
-  <si>
     <t>EXIGENCES Minimales</t>
   </si>
   <si>
@@ -120,20 +101,20 @@
     <t>Le projet sera réalisé sur le logiciel NetBeans</t>
   </si>
   <si>
-    <t>Le projet sera codé grâce aux langages: html, css, javascript</t>
-  </si>
-  <si>
-    <t>Le projet sera versioné sous Git</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Le projet sera codé grâce aux langages: html, css, javascript,bootstrap</t>
+  </si>
+  <si>
+    <t>Le projet sera versioné sous Github</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -159,20 +140,12 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -183,12 +156,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -306,7 +273,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -323,23 +290,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -358,7 +314,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -730,7 +686,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -744,11 +700,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
@@ -757,7 +713,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -765,7 +721,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -774,7 +730,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -783,7 +739,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -792,7 +748,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -884,7 +840,7 @@
         <v>1</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="2:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -929,28 +885,28 @@
       <c r="C25" s="5"/>
     </row>
     <row r="26" spans="2:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="19"/>
-      <c r="C26" s="20"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="15"/>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="19"/>
-      <c r="C27" s="20"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="15"/>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="19"/>
-      <c r="C28" s="20"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="15"/>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B29" s="19"/>
-      <c r="C29" s="20"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="15"/>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B30" s="19"/>
-      <c r="C30" s="20"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="15"/>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B31" s="19"/>
-      <c r="C31" s="20"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -976,12 +932,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
@@ -1007,24 +963,24 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1040,7 +996,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -1058,28 +1014,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="28"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="23"/>
       <c r="H1" s="4"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="21" t="s">
-        <v>23</v>
+      <c r="D2" s="16" t="s">
+        <v>17</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>12</v>
@@ -1094,69 +1050,69 @@
     <row r="3" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
     </row>
     <row r="4" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
     </row>
     <row r="5" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
     </row>
     <row r="6" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
     </row>
     <row r="7" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
     </row>
     <row r="8" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D11" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" s="22">
+      <c r="D11" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="17">
         <f>SUM(E3:E7)</f>
         <v>0</v>
       </c>
@@ -1168,250 +1124,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I29"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="2.7109375"/>
-    <col min="2" max="2" width="9.85546875"/>
-    <col min="3" max="3" width="103.5703125"/>
-    <col min="4" max="5" width="15.85546875"/>
-    <col min="6" max="6" width="20" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875"/>
-    <col min="8" max="1025" width="10.5703125"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-    </row>
-    <row r="4" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="14"/>
-      <c r="C4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-    </row>
-    <row r="5" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="2">
-        <f>1</f>
-        <v>1</v>
-      </c>
-      <c r="C5" s="5"/>
-    </row>
-    <row r="6" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="2">
-        <f>B5+1</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="2">
-        <f t="shared" ref="B7:B10" si="0">B6+1</f>
-        <v>3</v>
-      </c>
-      <c r="C7" s="4"/>
-    </row>
-    <row r="8" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="2">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="C8" s="4"/>
-    </row>
-    <row r="9" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="2">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C9" s="4"/>
-    </row>
-    <row r="10" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="2">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-    </row>
-    <row r="11" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="14"/>
-      <c r="C11" s="3"/>
-    </row>
-    <row r="12" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="2">
-        <f>B10+1</f>
-        <v>7</v>
-      </c>
-      <c r="C12" s="3"/>
-    </row>
-    <row r="13" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="2">
-        <f t="shared" ref="B13:B21" si="1">B12+1</f>
-        <v>8</v>
-      </c>
-      <c r="C13" s="3"/>
-    </row>
-    <row r="14" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="2">
-        <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="C14" s="3"/>
-    </row>
-    <row r="15" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="2">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="C15" s="4"/>
-    </row>
-    <row r="16" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="2">
-        <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-      <c r="C16" s="4"/>
-    </row>
-    <row r="17" spans="2:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="2">
-        <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="C17" s="4"/>
-    </row>
-    <row r="18" spans="2:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="2">
-        <f t="shared" si="1"/>
-        <v>13</v>
-      </c>
-      <c r="C18" s="4"/>
-    </row>
-    <row r="19" spans="2:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="2">
-        <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-      <c r="C19" s="4"/>
-    </row>
-    <row r="20" spans="2:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="2">
-        <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-      <c r="C20" s="4"/>
-    </row>
-    <row r="21" spans="2:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="2">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="C21" s="4"/>
-    </row>
-    <row r="22" spans="2:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C22" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="12">
-        <f>B21+1</f>
-        <v>17</v>
-      </c>
-      <c r="C23" s="5"/>
-    </row>
-    <row r="24" spans="2:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="12">
-        <f>B23+1</f>
-        <v>18</v>
-      </c>
-      <c r="C24" s="5"/>
-    </row>
-    <row r="25" spans="2:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="12">
-        <f>B24+1</f>
-        <v>19</v>
-      </c>
-      <c r="C25" s="5"/>
-    </row>
-    <row r="26" spans="2:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="12">
-        <f>B25+1</f>
-        <v>20</v>
-      </c>
-      <c r="C26" s="5"/>
-    </row>
-    <row r="27" spans="2:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="12">
-        <f>B26+1</f>
-        <v>21</v>
-      </c>
-      <c r="C27" s="5"/>
-    </row>
-    <row r="28" spans="2:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="12">
-        <f>B27+1</f>
-        <v>22</v>
-      </c>
-      <c r="C28" s="5"/>
-    </row>
-    <row r="29" spans="2:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>